<commit_message>
fix(63850): Corrige cálculo campo 15 - Saldo reprogramado próximo período
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_relatorio_dre_sme.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_relatorio_dre_sme.xlsx
@@ -76,53 +76,13 @@
     <t xml:space="preserve">12 - Demais créditos</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">13 - Valor total </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(07+09+10+11+12)</t>
-    </r>
+    <t xml:space="preserve">13 - Valor total</t>
   </si>
   <si>
     <t xml:space="preserve">14 - Despesa realizada</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">15 - Saldo reprogramado próximo período </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(07+09+10+11+12)</t>
-    </r>
+    <t xml:space="preserve">15 - Saldo reprogramado próximo período</t>
   </si>
   <si>
     <t xml:space="preserve">16 - Devolução ao tesouro</t>
@@ -261,27 +221,7 @@
     <t xml:space="preserve">39 - Despesa realizada</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">40 - Saldo </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(34+35+36+37+38-39)</t>
-    </r>
+    <t xml:space="preserve">40 – Saldo</t>
   </si>
   <si>
     <t xml:space="preserve">41 - Devolução ao tesouro</t>
@@ -432,7 +372,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -500,12 +440,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i val="true"/>
       <sz val="8"/>
       <color rgb="FF000000"/>
@@ -522,15 +456,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="10"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
+      <i val="true"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -756,7 +690,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="109">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -797,30 +731,26 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -833,31 +763,27 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -877,64 +803,60 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -997,7 +919,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1017,7 +939,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1025,7 +947,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1049,7 +971,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1069,7 +991,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1077,7 +999,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1093,7 +1015,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1105,7 +1027,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1117,7 +1039,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1125,7 +1047,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1145,11 +1067,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1201,7 +1123,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1289,9 +1211,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>40680</xdr:colOff>
+      <xdr:colOff>40320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>330480</xdr:rowOff>
+      <xdr:rowOff>330120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1305,7 +1227,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="646920" cy="559080"/>
+          <a:ext cx="646560" cy="558720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1321,17 +1243,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E28" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22"/>
@@ -1345,10 +1267,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1434,14 +1356,14 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="12"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
@@ -1449,7 +1371,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1457,263 +1379,263 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="27"/>
-      <c r="L13" s="26" t="s">
+      <c r="K13" s="25"/>
+      <c r="L13" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="28"/>
-      <c r="N13" s="29"/>
-    </row>
-    <row r="14" s="35" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="M13" s="26"/>
+      <c r="N13" s="27"/>
+    </row>
+    <row r="14" s="33" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-    </row>
-    <row r="15" s="35" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+    </row>
+    <row r="15" s="33" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-    </row>
-    <row r="16" s="35" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+    </row>
+    <row r="16" s="33" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-    </row>
-    <row r="17" s="35" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+    </row>
+    <row r="17" s="33" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-    </row>
-    <row r="18" s="35" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="41"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+    </row>
+    <row r="18" s="33" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="39"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="45"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="46"/>
-      <c r="C21" s="24"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
@@ -1729,140 +1651,140 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-    </row>
-    <row r="24" s="49" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="47" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+    </row>
+    <row r="24" s="46" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="47" t="s">
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-    </row>
-    <row r="25" s="51" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="50" t="s">
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+    </row>
+    <row r="25" s="48" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="26" t="s">
+      <c r="B25" s="47"/>
+      <c r="C25" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="48"/>
-      <c r="G25" s="26" t="s">
+      <c r="F25" s="45"/>
+      <c r="G25" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="26" t="s">
+      <c r="H25" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="I25" s="26" t="s">
+      <c r="I25" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="26" t="s">
+      <c r="K25" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="L25" s="26" t="s">
+      <c r="L25" s="24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" s="49" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="52"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-    </row>
-    <row r="27" s="49" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="55"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-    </row>
-    <row r="28" s="49" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26" t="s">
+    <row r="26" s="46" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+    </row>
+    <row r="27" s="46" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+    </row>
+    <row r="28" s="46" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
+      <c r="C28" s="12"/>
+      <c r="D28" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-    </row>
-    <row r="29" s="49" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="58" t="n">
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+    </row>
+    <row r="29" s="46" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-    </row>
-    <row r="30" s="49" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+    </row>
+    <row r="30" s="46" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
@@ -1877,298 +1799,298 @@
       <c r="K31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="60"/>
-    </row>
-    <row r="33" s="63" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="61" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="57"/>
+    </row>
+    <row r="33" s="60" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="62" t="s">
+      <c r="C33" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="61" t="s">
+      <c r="D33" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="61" t="s">
+      <c r="E33" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="61" t="s">
+      <c r="F33" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="G33" s="61" t="s">
+      <c r="G33" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="H33" s="61" t="s">
+      <c r="H33" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="I33" s="61" t="s">
+      <c r="I33" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="J33" s="61" t="s">
+      <c r="J33" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="K33" s="61" t="s">
+      <c r="K33" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="L33" s="62" t="s">
+      <c r="L33" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="O33" s="64"/>
+      <c r="O33" s="61"/>
     </row>
     <row r="34" s="9" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="65"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="67" t="s">
+      <c r="A34" s="62"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="71"/>
-      <c r="M34" s="72"/>
-      <c r="N34" s="72"/>
-      <c r="O34" s="64"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="69"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="61"/>
     </row>
     <row r="35" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="73" t="n">
+      <c r="A35" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="B35" s="74"/>
-      <c r="C35" s="30" t="s">
+      <c r="B35" s="71"/>
+      <c r="C35" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="75"/>
-      <c r="J35" s="75"/>
-      <c r="K35" s="77"/>
-      <c r="L35" s="71"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="68"/>
     </row>
     <row r="36" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="78"/>
-      <c r="B36" s="79"/>
-      <c r="C36" s="80" t="s">
+      <c r="A36" s="75"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="81"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="71"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="68"/>
     </row>
     <row r="37" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="84"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="67" t="s">
+      <c r="A37" s="81"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="86"/>
-      <c r="L37" s="71"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="68"/>
     </row>
     <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="87"/>
-      <c r="B38" s="88" t="s">
+      <c r="A38" s="84"/>
+      <c r="B38" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="89"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="71"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="68"/>
     </row>
     <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="90"/>
-      <c r="B39" s="91"/>
-      <c r="C39" s="80" t="s">
+      <c r="A39" s="87"/>
+      <c r="B39" s="88"/>
+      <c r="C39" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="82"/>
-      <c r="J39" s="81"/>
-      <c r="K39" s="83"/>
-      <c r="L39" s="71"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="79"/>
+      <c r="J39" s="78"/>
+      <c r="K39" s="80"/>
+      <c r="L39" s="68"/>
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="92"/>
-      <c r="B40" s="93"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="94"/>
-      <c r="E40" s="94"/>
-      <c r="F40" s="94"/>
-      <c r="G40" s="94"/>
-      <c r="H40" s="94"/>
-      <c r="I40" s="94"/>
-      <c r="J40" s="94"/>
-      <c r="K40" s="95"/>
-    </row>
-    <row r="41" s="49" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="50" t="s">
+      <c r="A40" s="89"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="91"/>
+      <c r="E40" s="91"/>
+      <c r="F40" s="91"/>
+      <c r="G40" s="91"/>
+      <c r="H40" s="91"/>
+      <c r="I40" s="91"/>
+      <c r="J40" s="91"/>
+      <c r="K40" s="92"/>
+    </row>
+    <row r="41" s="46" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="19" t="s">
+      <c r="B41" s="47"/>
+      <c r="C41" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19" t="s">
+      <c r="D41" s="12"/>
+      <c r="E41" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19" t="s">
+      <c r="F41" s="12"/>
+      <c r="G41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-    </row>
-    <row r="42" s="49" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="96" t="s">
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+    </row>
+    <row r="42" s="46" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="96"/>
-      <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="96"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="96"/>
-      <c r="I42" s="96"/>
-      <c r="J42" s="96"/>
-      <c r="K42" s="96"/>
-      <c r="L42" s="96"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="93"/>
+      <c r="D42" s="93"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="93"/>
+      <c r="G42" s="93"/>
+      <c r="H42" s="93"/>
+      <c r="I42" s="93"/>
+      <c r="J42" s="93"/>
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="97"/>
-      <c r="B43" s="97"/>
-      <c r="C43" s="98"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="99"/>
-      <c r="F43" s="99"/>
-      <c r="G43" s="100"/>
-      <c r="H43" s="100"/>
-      <c r="I43" s="100"/>
-      <c r="J43" s="100"/>
-      <c r="K43" s="100"/>
-      <c r="L43" s="100"/>
+      <c r="A43" s="94"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="95"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="96"/>
+      <c r="G43" s="97"/>
+      <c r="H43" s="97"/>
+      <c r="I43" s="97"/>
+      <c r="J43" s="97"/>
+      <c r="K43" s="97"/>
+      <c r="L43" s="97"/>
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="97"/>
-      <c r="B44" s="97"/>
-      <c r="C44" s="98"/>
-      <c r="D44" s="98"/>
-      <c r="E44" s="99"/>
-      <c r="F44" s="99"/>
-      <c r="G44" s="100"/>
-      <c r="H44" s="100"/>
-      <c r="I44" s="100"/>
-      <c r="J44" s="100"/>
-      <c r="K44" s="100"/>
-      <c r="L44" s="100"/>
-    </row>
-    <row r="45" s="49" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="96" t="s">
+      <c r="A44" s="94"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="96"/>
+      <c r="G44" s="97"/>
+      <c r="H44" s="97"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="97"/>
+      <c r="K44" s="97"/>
+      <c r="L44" s="97"/>
+    </row>
+    <row r="45" s="46" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="96"/>
-      <c r="C45" s="96"/>
-      <c r="D45" s="96"/>
-      <c r="E45" s="96"/>
-      <c r="F45" s="96"/>
-      <c r="G45" s="96"/>
-      <c r="H45" s="96"/>
-      <c r="I45" s="96"/>
-      <c r="J45" s="96"/>
-      <c r="K45" s="96"/>
-      <c r="L45" s="96"/>
+      <c r="B45" s="93"/>
+      <c r="C45" s="93"/>
+      <c r="D45" s="93"/>
+      <c r="E45" s="93"/>
+      <c r="F45" s="93"/>
+      <c r="G45" s="93"/>
+      <c r="H45" s="93"/>
+      <c r="I45" s="93"/>
+      <c r="J45" s="93"/>
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="97"/>
-      <c r="B46" s="97"/>
-      <c r="C46" s="98"/>
-      <c r="D46" s="98"/>
-      <c r="E46" s="99"/>
-      <c r="F46" s="99"/>
-      <c r="G46" s="100"/>
-      <c r="H46" s="100"/>
-      <c r="I46" s="100"/>
-      <c r="J46" s="100"/>
-      <c r="K46" s="100"/>
-      <c r="L46" s="100"/>
+      <c r="A46" s="94"/>
+      <c r="B46" s="94"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="97"/>
+      <c r="H46" s="97"/>
+      <c r="I46" s="97"/>
+      <c r="J46" s="97"/>
+      <c r="K46" s="97"/>
+      <c r="L46" s="97"/>
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="97"/>
-      <c r="B47" s="97"/>
-      <c r="C47" s="98"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="99"/>
-      <c r="F47" s="99"/>
-      <c r="G47" s="100"/>
-      <c r="H47" s="100"/>
-      <c r="I47" s="100"/>
-      <c r="J47" s="100"/>
-      <c r="K47" s="100"/>
-      <c r="L47" s="100"/>
+      <c r="A47" s="94"/>
+      <c r="B47" s="94"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="96"/>
+      <c r="F47" s="96"/>
+      <c r="G47" s="97"/>
+      <c r="H47" s="97"/>
+      <c r="I47" s="97"/>
+      <c r="J47" s="97"/>
+      <c r="K47" s="97"/>
+      <c r="L47" s="97"/>
     </row>
     <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="24"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
@@ -2184,86 +2106,86 @@
       <c r="K49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
-      <c r="K50" s="15"/>
-      <c r="L50" s="15"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
     </row>
     <row r="51" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="101" t="s">
+      <c r="A51" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="102"/>
-      <c r="C51" s="102"/>
-      <c r="D51" s="102"/>
-      <c r="E51" s="102"/>
-      <c r="F51" s="102"/>
-      <c r="G51" s="102"/>
-      <c r="H51" s="102"/>
-      <c r="I51" s="102"/>
-      <c r="J51" s="102"/>
-      <c r="K51" s="102"/>
-      <c r="L51" s="103"/>
+      <c r="B51" s="99"/>
+      <c r="C51" s="99"/>
+      <c r="D51" s="99"/>
+      <c r="E51" s="99"/>
+      <c r="F51" s="99"/>
+      <c r="G51" s="99"/>
+      <c r="H51" s="99"/>
+      <c r="I51" s="99"/>
+      <c r="J51" s="99"/>
+      <c r="K51" s="99"/>
+      <c r="L51" s="100"/>
     </row>
     <row r="52" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="104" t="s">
+      <c r="A52" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="94"/>
-      <c r="C52" s="94"/>
-      <c r="D52" s="94"/>
-      <c r="E52" s="94"/>
-      <c r="F52" s="94"/>
-      <c r="G52" s="94"/>
-      <c r="H52" s="94"/>
-      <c r="I52" s="94"/>
-      <c r="J52" s="94"/>
-      <c r="K52" s="94"/>
-      <c r="L52" s="105"/>
+      <c r="B52" s="91"/>
+      <c r="C52" s="91"/>
+      <c r="D52" s="91"/>
+      <c r="E52" s="91"/>
+      <c r="F52" s="91"/>
+      <c r="G52" s="91"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="91"/>
+      <c r="K52" s="91"/>
+      <c r="L52" s="102"/>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="106"/>
-      <c r="B53" s="94"/>
-      <c r="C53" s="94"/>
-      <c r="D53" s="94"/>
-      <c r="E53" s="94"/>
-      <c r="F53" s="94"/>
-      <c r="G53" s="94"/>
-      <c r="H53" s="94"/>
-      <c r="I53" s="94"/>
-      <c r="J53" s="94"/>
-      <c r="K53" s="94"/>
-      <c r="L53" s="105"/>
+      <c r="A53" s="103"/>
+      <c r="B53" s="91"/>
+      <c r="C53" s="91"/>
+      <c r="D53" s="91"/>
+      <c r="E53" s="91"/>
+      <c r="F53" s="91"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="91"/>
+      <c r="I53" s="91"/>
+      <c r="J53" s="91"/>
+      <c r="K53" s="91"/>
+      <c r="L53" s="102"/>
     </row>
     <row r="54" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="107" t="s">
+      <c r="A54" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="107"/>
-      <c r="C54" s="107"/>
-      <c r="D54" s="108"/>
-      <c r="E54" s="109" t="s">
+      <c r="B54" s="104"/>
+      <c r="C54" s="104"/>
+      <c r="D54" s="105"/>
+      <c r="E54" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="F54" s="109"/>
-      <c r="G54" s="109"/>
-      <c r="H54" s="108"/>
-      <c r="I54" s="109" t="s">
+      <c r="F54" s="106"/>
+      <c r="G54" s="106"/>
+      <c r="H54" s="105"/>
+      <c r="I54" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="J54" s="109"/>
-      <c r="K54" s="109"/>
-      <c r="L54" s="110"/>
+      <c r="J54" s="106"/>
+      <c r="K54" s="106"/>
+      <c r="L54" s="107"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9"/>
@@ -2284,7 +2206,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="111"/>
+      <c r="A60" s="108"/>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fix(63850): Corrige exibição dos campos 27, 28 e 42
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_relatorio_dre_sme.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_relatorio_dre_sme.xlsx
@@ -1200,60 +1200,18 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>66600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>40320</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>330120</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Imagem 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="66600" y="152280"/>
-          <a:ext cx="646560" cy="558720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1048576"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E28" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I40" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P54" activeCellId="0" sqref="P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22"/>
@@ -1273,7 +1231,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1286,7 +1244,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1320,7 +1278,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
@@ -1802,16 +1760,16 @@
       <c r="A32" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
       <c r="L32" s="57"/>
     </row>
     <row r="33" s="60" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1870,7 +1828,7 @@
       <c r="L34" s="68"/>
       <c r="M34" s="69"/>
       <c r="N34" s="69"/>
-      <c r="O34" s="61"/>
+      <c r="O34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="70" t="n">
@@ -2092,7 +2050,7 @@
       <c r="J48" s="22"/>
       <c r="K48" s="22"/>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2153,7 +2111,7 @@
       <c r="K52" s="91"/>
       <c r="L52" s="102"/>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="103"/>
       <c r="B53" s="91"/>
       <c r="C53" s="91"/>
@@ -2187,7 +2145,7 @@
       <c r="K54" s="106"/>
       <c r="L54" s="107"/>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -2208,13 +2166,6 @@
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="108"/>
     </row>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="57">
     <mergeCell ref="G2:K2"/>
@@ -2282,6 +2233,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>